<commit_message>
texto no cruza determinante-upload requirements
</commit_message>
<xml_diff>
--- a/Variables.xlsx
+++ b/Variables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEO_J\Desktop\POSPR_PRADERA\03_Desarrollos\textos_reporte_determinantes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LEO_J\Desktop\POSPR_PRADERA\03_Desarrollos\reporte_determinantes_usos_uaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{303BE382-983F-4834-9767-06CDBBA339AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92B2331-3BE8-4798-8B9E-6173400F300F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{60A766E9-BF47-4DF1-85FA-3B7576609285}"/>
+    <workbookView xWindow="20370" yWindow="-2070" windowWidth="21840" windowHeight="13140" xr2:uid="{60A766E9-BF47-4DF1-85FA-3B7576609285}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -649,7 +649,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>